<commit_message>
simulations and modifications to param estimates
</commit_message>
<xml_diff>
--- a/literature_extraction.xlsx
+++ b/literature_extraction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jower\OneDrive\Documents\GitHub\Species-Traits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2038" documentId="8_{8303F361-5CFA-49CF-93EB-E47B0D017CB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{45BAFCE0-C8F9-4312-9D84-0C6F00FCDB9E}"/>
+  <xr:revisionPtr revIDLastSave="2039" documentId="8_{8303F361-5CFA-49CF-93EB-E47B0D017CB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B3AAD7FE-04E4-4A37-8E34-2B4BFBBCA738}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{163C3060-5853-4BB6-B46C-A85E56A5A6D8}"/>
+    <workbookView xWindow="3555" yWindow="1575" windowWidth="23040" windowHeight="13170" activeTab="1" xr2:uid="{163C3060-5853-4BB6-B46C-A85E56A5A6D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2893,7 +2893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4942DADD-73DC-45E2-A058-0029641B6054}">
   <dimension ref="A1:G198"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
@@ -6338,9 +6338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C553106-9EFB-4C5F-86D3-BA2759CF7F90}">
   <dimension ref="A1:AM204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6351,6 +6351,7 @@
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" customWidth="1"/>
     <col min="16" max="16" width="17.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
     <col min="27" max="27" width="12.140625" customWidth="1"/>
     <col min="39" max="39" width="9.42578125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
feeding model adding random effect slope
</commit_message>
<xml_diff>
--- a/literature_extraction.xlsx
+++ b/literature_extraction.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jower\OneDrive\Documents\GitHub\Species-Traits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\OneDrive\Documents\GitHub\Species-Traits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3627" documentId="8_{8303F361-5CFA-49CF-93EB-E47B0D017CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA26B6B1-ABBB-49AF-B888-588EA6CF59CC}"/>
+  <xr:revisionPtr revIDLastSave="3630" documentId="8_{8303F361-5CFA-49CF-93EB-E47B0D017CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0AEAFDC1-1549-49FC-981C-81107BBD03C9}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="22635" windowHeight="12510" xr2:uid="{163C3060-5853-4BB6-B46C-A85E56A5A6D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{163C3060-5853-4BB6-B46C-A85E56A5A6D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3566" uniqueCount="1262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3567" uniqueCount="1263">
   <si>
     <t>Title</t>
   </si>
@@ -3819,6 +3819,9 @@
   </si>
   <si>
     <t>max uptake</t>
+  </si>
+  <si>
+    <t>also has survival curves, feeding only reported on cyano??</t>
   </si>
 </sst>
 </file>
@@ -4218,8 +4221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4942DADD-73DC-45E2-A058-0029641B6054}">
   <dimension ref="A1:G298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="B221" sqref="B221"/>
+    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
+      <selection activeCell="E290" sqref="E290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9114,21 +9117,24 @@
         <v>245</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A284" s="10" t="s">
+    <row r="284" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="12" t="s">
         <v>1199</v>
       </c>
-      <c r="B284" s="2" t="s">
+      <c r="B284" s="5" t="s">
         <v>1200</v>
       </c>
-      <c r="C284" s="2" t="s">
+      <c r="C284" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="D284" s="2" t="s">
+      <c r="D284" s="5" t="s">
         <v>687</v>
       </c>
-      <c r="E284" s="2" t="s">
+      <c r="E284" s="5" t="s">
         <v>1042</v>
+      </c>
+      <c r="F284" s="5" t="s">
+        <v>1262</v>
       </c>
     </row>
     <row r="285" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>